<commit_message>
various changes with implementing jquery
</commit_message>
<xml_diff>
--- a/Documents/GENERAL LEDGER TEMPLATE.xlsx
+++ b/Documents/GENERAL LEDGER TEMPLATE.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lloydnicholson/Documents/GitHub/accounting-app/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E63B0F-AB1A-D949-8631-AE5AECE3790B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FE270D-0463-1244-91EC-7AA527DA4189}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{8DDA6EC7-4F49-7D46-9ABB-4C033F15353F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="20480" xr2:uid="{8DDA6EC7-4F49-7D46-9ABB-4C033F15353F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="38">
   <si>
     <t>Day</t>
   </si>
@@ -42,9 +42,6 @@
     <t>BALANCE SHEET SECTION</t>
   </si>
   <si>
-    <t xml:space="preserve">                         GENERAL LEDGER OF </t>
-  </si>
-  <si>
     <t>Month</t>
   </si>
   <si>
@@ -63,10 +60,85 @@
     <t>RENT EXPENSE</t>
   </si>
   <si>
-    <t>NAME:</t>
-  </si>
-  <si>
     <t>CAPITAL</t>
+  </si>
+  <si>
+    <t>NAME: Activity 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                         GENERAL LEDGER OF URBAN FITNESS FOR FEBRUARY 2017</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Capital</t>
+  </si>
+  <si>
+    <t>CRJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feb </t>
+  </si>
+  <si>
+    <t>Bank</t>
+  </si>
+  <si>
+    <t>Equipment</t>
+  </si>
+  <si>
+    <t>CPJ</t>
+  </si>
+  <si>
+    <t>EQUIPMENT</t>
+  </si>
+  <si>
+    <t>Rent expense</t>
+  </si>
+  <si>
+    <t>Current income</t>
+  </si>
+  <si>
+    <t>Wages</t>
+  </si>
+  <si>
+    <t>WAGES</t>
+  </si>
+  <si>
+    <t>Drawings</t>
+  </si>
+  <si>
+    <t>DRAWINGS</t>
+  </si>
+  <si>
+    <t>Water and Electricity</t>
+  </si>
+  <si>
+    <t>WATER AND ELECTRICITY</t>
+  </si>
+  <si>
+    <t>Telephone</t>
+  </si>
+  <si>
+    <t>TELEPHONE</t>
+  </si>
+  <si>
+    <t>Stationery</t>
+  </si>
+  <si>
+    <t>STATIONERY</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>c/d</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>b/d</t>
   </si>
 </sst>
 </file>
@@ -113,7 +185,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -415,11 +487,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -452,6 +550,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -464,15 +574,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -482,10 +583,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -805,8 +910,8 @@
   </sheetPr>
   <dimension ref="A2:W83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="200" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -832,71 +937,71 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" ht="34" x14ac:dyDescent="0.4">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
     </row>
     <row r="5" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:23" ht="25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="25"/>
-      <c r="N6" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
-      <c r="T6" s="24"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="24"/>
-      <c r="W6" s="25"/>
+      <c r="B6" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="29"/>
+      <c r="N6" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
+      <c r="R6" s="28"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="28"/>
+      <c r="U6" s="28"/>
+      <c r="V6" s="28"/>
+      <c r="W6" s="29"/>
     </row>
     <row r="7" spans="1:23" ht="25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="31"/>
-      <c r="N7" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="30"/>
-      <c r="S7" s="30"/>
-      <c r="T7" s="30"/>
-      <c r="U7" s="30"/>
-      <c r="V7" s="30"/>
-      <c r="W7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="32"/>
+      <c r="N7" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="31"/>
+      <c r="T7" s="31"/>
+      <c r="U7" s="31"/>
+      <c r="V7" s="31"/>
+      <c r="W7" s="32"/>
     </row>
     <row r="8" spans="1:23" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="19"/>
@@ -921,35 +1026,35 @@
       <c r="W8" s="21"/>
     </row>
     <row r="9" spans="1:23" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="28"/>
-      <c r="N9" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="27"/>
-      <c r="R9" s="27"/>
-      <c r="S9" s="27"/>
-      <c r="T9" s="27"/>
-      <c r="U9" s="27"/>
-      <c r="V9" s="27"/>
-      <c r="W9" s="28"/>
+      <c r="B9" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="25"/>
+      <c r="N9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
+      <c r="V9" s="24"/>
+      <c r="W9" s="25"/>
     </row>
     <row r="10" spans="1:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
+      <c r="A10" s="1"/>
       <c r="B10" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>0</v>
@@ -964,7 +1069,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>0</v>
@@ -980,7 +1085,7 @@
       </c>
       <c r="L10" s="1"/>
       <c r="N10" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O10" s="11" t="s">
         <v>0</v>
@@ -995,7 +1100,7 @@
         <v>3</v>
       </c>
       <c r="S10" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T10" s="11" t="s">
         <v>0</v>
@@ -1011,60 +1116,128 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="10"/>
+      <c r="B11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="9">
+        <v>1</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="33">
+        <v>1000000</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="9">
+        <v>4</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="34">
+        <v>800000</v>
+      </c>
       <c r="N11" s="8"/>
       <c r="O11" s="9"/>
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
       <c r="R11" s="16"/>
-      <c r="S11" s="13"/>
-      <c r="T11" s="9"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="9"/>
-      <c r="W11" s="10"/>
+      <c r="S11" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="T11" s="9">
+        <v>6</v>
+      </c>
+      <c r="U11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="V11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="W11" s="34">
+        <v>112500</v>
+      </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B12" s="3"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="17"/>
+      <c r="C12" s="2">
+        <v>6</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="36">
+        <v>112500</v>
+      </c>
       <c r="G12" s="14"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="4"/>
+      <c r="I12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="35">
+        <v>35000</v>
+      </c>
       <c r="N12" s="3"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="17"/>
       <c r="S12" s="14"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
-      <c r="W12" s="4"/>
+      <c r="T12" s="2">
+        <v>19</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="V12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="W12" s="35">
+        <v>10120</v>
+      </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B13" s="3"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="17"/>
+      <c r="C13" s="2">
+        <v>19</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="36">
+        <v>10120</v>
+      </c>
       <c r="G13" s="14"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="4"/>
+      <c r="H13" s="2">
+        <v>10</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="35">
+        <v>3000</v>
+      </c>
       <c r="N13" s="3"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
@@ -1079,14 +1252,28 @@
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B14" s="3"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="17"/>
+      <c r="D14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="36">
+        <v>200000</v>
+      </c>
       <c r="G14" s="14"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="4"/>
+      <c r="H14" s="2">
+        <v>12</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="35">
+        <v>19000</v>
+      </c>
       <c r="N14" s="3"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
@@ -1105,10 +1292,18 @@
       <c r="E15" s="2"/>
       <c r="F15" s="17"/>
       <c r="G15" s="14"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="4"/>
+      <c r="H15" s="2">
+        <v>15</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" s="35">
+        <v>6000</v>
+      </c>
       <c r="N15" s="3"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
@@ -1127,10 +1322,18 @@
       <c r="E16" s="2"/>
       <c r="F16" s="17"/>
       <c r="G16" s="14"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="4"/>
+      <c r="H16" s="2">
+        <v>16</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="35">
+        <v>2300</v>
+      </c>
       <c r="N16" s="3"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
@@ -1149,10 +1352,18 @@
       <c r="E17" s="2"/>
       <c r="F17" s="17"/>
       <c r="G17" s="14"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="4"/>
+      <c r="H17" s="2">
+        <v>21</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="35">
+        <v>1890</v>
+      </c>
       <c r="N17" s="5"/>
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
@@ -1171,10 +1382,18 @@
       <c r="E18" s="2"/>
       <c r="F18" s="17"/>
       <c r="G18" s="14"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="4"/>
+      <c r="H18" s="2">
+        <v>23</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="4">
+        <v>610</v>
+      </c>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
@@ -1183,10 +1402,18 @@
       <c r="E19" s="2"/>
       <c r="F19" s="17"/>
       <c r="G19" s="14"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="4"/>
+      <c r="H19" s="2">
+        <v>25</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K19" s="35">
+        <v>3000</v>
+      </c>
     </row>
     <row r="20" spans="2:23" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3"/>
@@ -1195,58 +1422,84 @@
       <c r="E20" s="2"/>
       <c r="F20" s="17"/>
       <c r="G20" s="14"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="4"/>
-      <c r="N20" s="32"/>
-      <c r="O20" s="32"/>
-      <c r="P20" s="32"/>
-      <c r="Q20" s="32"/>
-      <c r="R20" s="32"/>
-      <c r="S20" s="32"/>
-      <c r="T20" s="32"/>
-      <c r="U20" s="32"/>
-      <c r="V20" s="32"/>
-      <c r="W20" s="32"/>
+      <c r="H20" s="2">
+        <v>28</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K20" s="35">
+        <f>K21-SUM(K11:K19)</f>
+        <v>451820</v>
+      </c>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="22"/>
+      <c r="R20" s="22"/>
+      <c r="S20" s="22"/>
+      <c r="T20" s="22"/>
+      <c r="U20" s="22"/>
+      <c r="V20" s="22"/>
+      <c r="W20" s="22"/>
     </row>
     <row r="21" spans="2:23" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="3"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="17"/>
+      <c r="F21" s="37">
+        <f>SUM(F11:F14)</f>
+        <v>1322620</v>
+      </c>
       <c r="G21" s="14"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="4"/>
-      <c r="N21" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="O21" s="27"/>
-      <c r="P21" s="27"/>
-      <c r="Q21" s="27"/>
-      <c r="R21" s="27"/>
-      <c r="S21" s="27"/>
-      <c r="T21" s="27"/>
-      <c r="U21" s="27"/>
-      <c r="V21" s="27"/>
-      <c r="W21" s="28"/>
+      <c r="K21" s="39">
+        <f>F21</f>
+        <v>1322620</v>
+      </c>
+      <c r="N21" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="24"/>
+      <c r="S21" s="24"/>
+      <c r="T21" s="24"/>
+      <c r="U21" s="24"/>
+      <c r="V21" s="24"/>
+      <c r="W21" s="25"/>
     </row>
     <row r="22" spans="2:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="18"/>
+      <c r="B22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="6">
+        <v>1</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="40">
+        <f>K20</f>
+        <v>451820</v>
+      </c>
       <c r="G22" s="15"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
-      <c r="K22" s="7"/>
+      <c r="K22" s="38"/>
       <c r="N22" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O22" s="11" t="s">
         <v>0</v>
@@ -1261,7 +1514,7 @@
         <v>3</v>
       </c>
       <c r="S22" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T22" s="11" t="s">
         <v>0</v>
@@ -1289,18 +1542,18 @@
       <c r="W23" s="10"/>
     </row>
     <row r="24" spans="2:23" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="28"/>
+      <c r="B24" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="25"/>
       <c r="N24" s="3"/>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
@@ -1314,7 +1567,7 @@
     </row>
     <row r="25" spans="2:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>0</v>
@@ -1329,7 +1582,7 @@
         <v>3</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H25" s="11" t="s">
         <v>0</v>
@@ -1360,11 +1613,21 @@
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="16"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="10"/>
+      <c r="G26" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="9">
+        <v>1</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" s="34">
+        <v>1000000</v>
+      </c>
       <c r="N26" s="3"/>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
@@ -1383,10 +1646,18 @@
       <c r="E27" s="2"/>
       <c r="F27" s="17"/>
       <c r="G27" s="14"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="4"/>
+      <c r="H27" s="2">
+        <v>19</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K27" s="35">
+        <v>200000</v>
+      </c>
       <c r="N27" s="3"/>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
@@ -1465,18 +1736,18 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="4"/>
-      <c r="N31" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="O31" s="27"/>
-      <c r="P31" s="27"/>
-      <c r="Q31" s="27"/>
-      <c r="R31" s="27"/>
-      <c r="S31" s="27"/>
-      <c r="T31" s="27"/>
-      <c r="U31" s="27"/>
-      <c r="V31" s="27"/>
-      <c r="W31" s="28"/>
+      <c r="N31" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="O31" s="24"/>
+      <c r="P31" s="24"/>
+      <c r="Q31" s="24"/>
+      <c r="R31" s="24"/>
+      <c r="S31" s="24"/>
+      <c r="T31" s="24"/>
+      <c r="U31" s="24"/>
+      <c r="V31" s="24"/>
+      <c r="W31" s="25"/>
     </row>
     <row r="32" spans="2:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
@@ -1490,7 +1761,7 @@
       <c r="J32" s="6"/>
       <c r="K32" s="7"/>
       <c r="N32" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O32" s="11" t="s">
         <v>0</v>
@@ -1505,7 +1776,7 @@
         <v>3</v>
       </c>
       <c r="S32" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T32" s="11" t="s">
         <v>0</v>
@@ -1521,11 +1792,21 @@
       </c>
     </row>
     <row r="33" spans="2:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="N33" s="8"/>
-      <c r="O33" s="9"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="9"/>
-      <c r="R33" s="16"/>
+      <c r="N33" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="O33" s="9">
+        <v>4</v>
+      </c>
+      <c r="P33" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q33" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="R33" s="33">
+        <v>35000</v>
+      </c>
       <c r="S33" s="13"/>
       <c r="T33" s="9"/>
       <c r="U33" s="9"/>
@@ -1533,16 +1814,18 @@
       <c r="W33" s="10"/>
     </row>
     <row r="34" spans="2:23" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="26"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="27"/>
-      <c r="J34" s="27"/>
-      <c r="K34" s="28"/>
+      <c r="B34" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="25"/>
       <c r="N34" s="3"/>
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
@@ -1556,7 +1839,7 @@
     </row>
     <row r="35" spans="2:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C35" s="11" t="s">
         <v>0</v>
@@ -1571,7 +1854,7 @@
         <v>3</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H35" s="11" t="s">
         <v>0</v>
@@ -1597,11 +1880,21 @@
       <c r="W35" s="4"/>
     </row>
     <row r="36" spans="2:23" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="8"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="16"/>
+      <c r="B36" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="9">
+        <v>4</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" s="33">
+        <v>800000</v>
+      </c>
       <c r="G36" s="13"/>
       <c r="H36" s="9"/>
       <c r="I36" s="9"/>
@@ -1620,10 +1913,18 @@
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B37" s="3"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="17"/>
+      <c r="C37" s="2">
+        <v>12</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" s="36">
+        <v>19000</v>
+      </c>
       <c r="G37" s="14"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
@@ -1707,16 +2008,18 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="4"/>
-      <c r="N41" s="26"/>
-      <c r="O41" s="27"/>
-      <c r="P41" s="27"/>
-      <c r="Q41" s="27"/>
-      <c r="R41" s="27"/>
-      <c r="S41" s="27"/>
-      <c r="T41" s="27"/>
-      <c r="U41" s="27"/>
-      <c r="V41" s="27"/>
-      <c r="W41" s="28"/>
+      <c r="N41" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="O41" s="24"/>
+      <c r="P41" s="24"/>
+      <c r="Q41" s="24"/>
+      <c r="R41" s="24"/>
+      <c r="S41" s="24"/>
+      <c r="T41" s="24"/>
+      <c r="U41" s="24"/>
+      <c r="V41" s="24"/>
+      <c r="W41" s="25"/>
     </row>
     <row r="42" spans="2:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B42" s="5"/>
@@ -1730,7 +2033,7 @@
       <c r="J42" s="6"/>
       <c r="K42" s="7"/>
       <c r="N42" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O42" s="11" t="s">
         <v>0</v>
@@ -1745,7 +2048,7 @@
         <v>3</v>
       </c>
       <c r="S42" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T42" s="11" t="s">
         <v>0</v>
@@ -1761,11 +2064,21 @@
       </c>
     </row>
     <row r="43" spans="2:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="N43" s="8"/>
-      <c r="O43" s="9"/>
-      <c r="P43" s="9"/>
-      <c r="Q43" s="9"/>
-      <c r="R43" s="16"/>
+      <c r="N43" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="O43" s="9">
+        <v>10</v>
+      </c>
+      <c r="P43" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q43" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="R43" s="33">
+        <v>3000</v>
+      </c>
       <c r="S43" s="13"/>
       <c r="T43" s="9"/>
       <c r="U43" s="9"/>
@@ -1773,21 +2086,31 @@
       <c r="W43" s="10"/>
     </row>
     <row r="44" spans="2:23" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="26"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="27"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
-      <c r="K44" s="28"/>
+      <c r="B44" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="24"/>
+      <c r="J44" s="24"/>
+      <c r="K44" s="25"/>
       <c r="N44" s="3"/>
-      <c r="O44" s="2"/>
-      <c r="P44" s="2"/>
-      <c r="Q44" s="2"/>
-      <c r="R44" s="17"/>
+      <c r="O44" s="2">
+        <v>25</v>
+      </c>
+      <c r="P44" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q44" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R44" s="36">
+        <v>3000</v>
+      </c>
       <c r="S44" s="14"/>
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
@@ -1796,7 +2119,7 @@
     </row>
     <row r="45" spans="2:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B45" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>0</v>
@@ -1811,7 +2134,7 @@
         <v>3</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H45" s="11" t="s">
         <v>0</v>
@@ -1837,11 +2160,21 @@
       <c r="W45" s="4"/>
     </row>
     <row r="46" spans="2:23" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="8"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="16"/>
+      <c r="B46" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" s="9">
+        <v>15</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" s="33">
+        <v>6000</v>
+      </c>
       <c r="G46" s="13"/>
       <c r="H46" s="9"/>
       <c r="I46" s="9"/>
@@ -1947,16 +2280,18 @@
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="4"/>
-      <c r="N51" s="26"/>
-      <c r="O51" s="27"/>
-      <c r="P51" s="27"/>
-      <c r="Q51" s="27"/>
-      <c r="R51" s="27"/>
-      <c r="S51" s="27"/>
-      <c r="T51" s="27"/>
-      <c r="U51" s="27"/>
-      <c r="V51" s="27"/>
-      <c r="W51" s="28"/>
+      <c r="N51" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="O51" s="24"/>
+      <c r="P51" s="24"/>
+      <c r="Q51" s="24"/>
+      <c r="R51" s="24"/>
+      <c r="S51" s="24"/>
+      <c r="T51" s="24"/>
+      <c r="U51" s="24"/>
+      <c r="V51" s="24"/>
+      <c r="W51" s="25"/>
     </row>
     <row r="52" spans="2:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B52" s="5"/>
@@ -1970,7 +2305,7 @@
       <c r="J52" s="6"/>
       <c r="K52" s="7"/>
       <c r="N52" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O52" s="11" t="s">
         <v>0</v>
@@ -1985,7 +2320,7 @@
         <v>3</v>
       </c>
       <c r="S52" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T52" s="11" t="s">
         <v>0</v>
@@ -2001,11 +2336,21 @@
       </c>
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="N53" s="3"/>
-      <c r="O53" s="2"/>
-      <c r="P53" s="2"/>
-      <c r="Q53" s="2"/>
-      <c r="R53" s="17"/>
+      <c r="N53" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O53" s="2">
+        <v>16</v>
+      </c>
+      <c r="P53" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q53" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R53" s="36">
+        <v>2300</v>
+      </c>
       <c r="S53" s="14"/>
       <c r="T53" s="2"/>
       <c r="U53" s="2"/>
@@ -2025,16 +2370,16 @@
       <c r="W54" s="4"/>
     </row>
     <row r="55" spans="2:23" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="26"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="27"/>
-      <c r="G55" s="27"/>
-      <c r="H55" s="27"/>
-      <c r="I55" s="27"/>
-      <c r="J55" s="27"/>
-      <c r="K55" s="28"/>
+      <c r="B55" s="23"/>
+      <c r="C55" s="24"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="24"/>
+      <c r="H55" s="24"/>
+      <c r="I55" s="24"/>
+      <c r="J55" s="24"/>
+      <c r="K55" s="25"/>
       <c r="N55" s="3"/>
       <c r="O55" s="2"/>
       <c r="P55" s="2"/>
@@ -2048,7 +2393,7 @@
     </row>
     <row r="56" spans="2:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B56" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C56" s="11" t="s">
         <v>0</v>
@@ -2063,7 +2408,7 @@
         <v>3</v>
       </c>
       <c r="G56" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H56" s="11" t="s">
         <v>0</v>
@@ -2111,16 +2456,18 @@
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
       <c r="K58" s="4"/>
-      <c r="N58" s="26"/>
-      <c r="O58" s="27"/>
-      <c r="P58" s="27"/>
-      <c r="Q58" s="27"/>
-      <c r="R58" s="27"/>
-      <c r="S58" s="27"/>
-      <c r="T58" s="27"/>
-      <c r="U58" s="27"/>
-      <c r="V58" s="27"/>
-      <c r="W58" s="28"/>
+      <c r="N58" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="O58" s="24"/>
+      <c r="P58" s="24"/>
+      <c r="Q58" s="24"/>
+      <c r="R58" s="24"/>
+      <c r="S58" s="24"/>
+      <c r="T58" s="24"/>
+      <c r="U58" s="24"/>
+      <c r="V58" s="24"/>
+      <c r="W58" s="25"/>
     </row>
     <row r="59" spans="2:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B59" s="3"/>
@@ -2134,7 +2481,7 @@
       <c r="J59" s="2"/>
       <c r="K59" s="4"/>
       <c r="N59" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O59" s="11" t="s">
         <v>0</v>
@@ -2149,7 +2496,7 @@
         <v>3</v>
       </c>
       <c r="S59" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T59" s="11" t="s">
         <v>0</v>
@@ -2175,11 +2522,21 @@
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
       <c r="K60" s="7"/>
-      <c r="N60" s="8"/>
-      <c r="O60" s="9"/>
-      <c r="P60" s="9"/>
-      <c r="Q60" s="9"/>
-      <c r="R60" s="16"/>
+      <c r="N60" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="O60" s="9">
+        <v>21</v>
+      </c>
+      <c r="P60" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q60" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="R60" s="33">
+        <v>1890</v>
+      </c>
       <c r="S60" s="13"/>
       <c r="T60" s="9"/>
       <c r="U60" s="9"/>
@@ -2199,16 +2556,16 @@
       <c r="W61" s="4"/>
     </row>
     <row r="62" spans="2:23" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="26"/>
-      <c r="C62" s="27"/>
-      <c r="D62" s="27"/>
-      <c r="E62" s="27"/>
-      <c r="F62" s="27"/>
-      <c r="G62" s="27"/>
-      <c r="H62" s="27"/>
-      <c r="I62" s="27"/>
-      <c r="J62" s="27"/>
-      <c r="K62" s="28"/>
+      <c r="B62" s="23"/>
+      <c r="C62" s="24"/>
+      <c r="D62" s="24"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="24"/>
+      <c r="H62" s="24"/>
+      <c r="I62" s="24"/>
+      <c r="J62" s="24"/>
+      <c r="K62" s="25"/>
       <c r="N62" s="3"/>
       <c r="O62" s="2"/>
       <c r="P62" s="2"/>
@@ -2222,7 +2579,7 @@
     </row>
     <row r="63" spans="2:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B63" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C63" s="11" t="s">
         <v>0</v>
@@ -2237,7 +2594,7 @@
         <v>3</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H63" s="11" t="s">
         <v>0</v>
@@ -2307,16 +2664,18 @@
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
       <c r="K66" s="4"/>
-      <c r="N66" s="26"/>
-      <c r="O66" s="27"/>
-      <c r="P66" s="27"/>
-      <c r="Q66" s="27"/>
-      <c r="R66" s="27"/>
-      <c r="S66" s="27"/>
-      <c r="T66" s="27"/>
-      <c r="U66" s="27"/>
-      <c r="V66" s="27"/>
-      <c r="W66" s="28"/>
+      <c r="N66" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="O66" s="24"/>
+      <c r="P66" s="24"/>
+      <c r="Q66" s="24"/>
+      <c r="R66" s="24"/>
+      <c r="S66" s="24"/>
+      <c r="T66" s="24"/>
+      <c r="U66" s="24"/>
+      <c r="V66" s="24"/>
+      <c r="W66" s="25"/>
     </row>
     <row r="67" spans="2:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B67" s="3"/>
@@ -2330,7 +2689,7 @@
       <c r="J67" s="2"/>
       <c r="K67" s="4"/>
       <c r="N67" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O67" s="11" t="s">
         <v>0</v>
@@ -2345,7 +2704,7 @@
         <v>3</v>
       </c>
       <c r="S67" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T67" s="11" t="s">
         <v>0</v>
@@ -2371,11 +2730,21 @@
       <c r="I68" s="6"/>
       <c r="J68" s="6"/>
       <c r="K68" s="7"/>
-      <c r="N68" s="8"/>
-      <c r="O68" s="9"/>
-      <c r="P68" s="9"/>
-      <c r="Q68" s="9"/>
-      <c r="R68" s="16"/>
+      <c r="N68" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="O68" s="9">
+        <v>23</v>
+      </c>
+      <c r="P68" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q68" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="R68" s="16">
+        <v>610</v>
+      </c>
       <c r="S68" s="13"/>
       <c r="T68" s="9"/>
       <c r="U68" s="9"/>
@@ -2395,16 +2764,16 @@
       <c r="W69" s="4"/>
     </row>
     <row r="70" spans="2:23" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="26"/>
-      <c r="C70" s="27"/>
-      <c r="D70" s="27"/>
-      <c r="E70" s="27"/>
-      <c r="F70" s="27"/>
-      <c r="G70" s="27"/>
-      <c r="H70" s="27"/>
-      <c r="I70" s="27"/>
-      <c r="J70" s="27"/>
-      <c r="K70" s="28"/>
+      <c r="B70" s="23"/>
+      <c r="C70" s="24"/>
+      <c r="D70" s="24"/>
+      <c r="E70" s="24"/>
+      <c r="F70" s="24"/>
+      <c r="G70" s="24"/>
+      <c r="H70" s="24"/>
+      <c r="I70" s="24"/>
+      <c r="J70" s="24"/>
+      <c r="K70" s="25"/>
       <c r="N70" s="3"/>
       <c r="O70" s="2"/>
       <c r="P70" s="2"/>
@@ -2418,7 +2787,7 @@
     </row>
     <row r="71" spans="2:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B71" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C71" s="11" t="s">
         <v>0</v>
@@ -2433,7 +2802,7 @@
         <v>3</v>
       </c>
       <c r="G71" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H71" s="11" t="s">
         <v>0</v>
@@ -2503,16 +2872,16 @@
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
       <c r="K74" s="4"/>
-      <c r="N74" s="26"/>
-      <c r="O74" s="27"/>
-      <c r="P74" s="27"/>
-      <c r="Q74" s="27"/>
-      <c r="R74" s="27"/>
-      <c r="S74" s="27"/>
-      <c r="T74" s="27"/>
-      <c r="U74" s="27"/>
-      <c r="V74" s="27"/>
-      <c r="W74" s="28"/>
+      <c r="N74" s="23"/>
+      <c r="O74" s="24"/>
+      <c r="P74" s="24"/>
+      <c r="Q74" s="24"/>
+      <c r="R74" s="24"/>
+      <c r="S74" s="24"/>
+      <c r="T74" s="24"/>
+      <c r="U74" s="24"/>
+      <c r="V74" s="24"/>
+      <c r="W74" s="25"/>
     </row>
     <row r="75" spans="2:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B75" s="5"/>
@@ -2526,7 +2895,7 @@
       <c r="J75" s="6"/>
       <c r="K75" s="7"/>
       <c r="N75" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O75" s="11" t="s">
         <v>0</v>
@@ -2541,7 +2910,7 @@
         <v>3</v>
       </c>
       <c r="S75" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T75" s="11" t="s">
         <v>0</v>
@@ -2569,16 +2938,16 @@
       <c r="W76" s="10"/>
     </row>
     <row r="77" spans="2:23" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="26"/>
-      <c r="C77" s="27"/>
-      <c r="D77" s="27"/>
-      <c r="E77" s="27"/>
-      <c r="F77" s="27"/>
-      <c r="G77" s="27"/>
-      <c r="H77" s="27"/>
-      <c r="I77" s="27"/>
-      <c r="J77" s="27"/>
-      <c r="K77" s="28"/>
+      <c r="B77" s="23"/>
+      <c r="C77" s="24"/>
+      <c r="D77" s="24"/>
+      <c r="E77" s="24"/>
+      <c r="F77" s="24"/>
+      <c r="G77" s="24"/>
+      <c r="H77" s="24"/>
+      <c r="I77" s="24"/>
+      <c r="J77" s="24"/>
+      <c r="K77" s="25"/>
       <c r="N77" s="3"/>
       <c r="O77" s="2"/>
       <c r="P77" s="2"/>
@@ -2592,7 +2961,7 @@
     </row>
     <row r="78" spans="2:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B78" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C78" s="11" t="s">
         <v>0</v>
@@ -2607,7 +2976,7 @@
         <v>3</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H78" s="11" t="s">
         <v>0</v>
@@ -2714,11 +3083,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B24:K24"/>
-    <mergeCell ref="B34:K34"/>
-    <mergeCell ref="B70:K70"/>
-    <mergeCell ref="B77:K77"/>
-    <mergeCell ref="N74:W74"/>
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="N6:W6"/>
     <mergeCell ref="N58:W58"/>
@@ -2735,6 +3099,11 @@
     <mergeCell ref="B6:K6"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="B9:K9"/>
+    <mergeCell ref="B24:K24"/>
+    <mergeCell ref="B34:K34"/>
+    <mergeCell ref="B70:K70"/>
+    <mergeCell ref="B77:K77"/>
+    <mergeCell ref="N74:W74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="68" fitToWidth="2" fitToHeight="4" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
changed back to original template format
</commit_message>
<xml_diff>
--- a/Documents/GENERAL LEDGER TEMPLATE.xlsx
+++ b/Documents/GENERAL LEDGER TEMPLATE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lloydnicholson/Documents/GitHub/accounting-app/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FE270D-0463-1244-91EC-7AA527DA4189}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7204F761-1C0D-EB43-BFC8-707A46086781}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="20480" xr2:uid="{8DDA6EC7-4F49-7D46-9ABB-4C033F15353F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="17540" xr2:uid="{8DDA6EC7-4F49-7D46-9ABB-4C033F15353F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="20">
   <si>
     <t>Day</t>
   </si>
@@ -69,76 +69,22 @@
     <t xml:space="preserve">                         GENERAL LEDGER OF URBAN FITNESS FOR FEBRUARY 2017</t>
   </si>
   <si>
-    <t>Feb</t>
-  </si>
-  <si>
-    <t>Capital</t>
-  </si>
-  <si>
-    <t>CRJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feb </t>
-  </si>
-  <si>
-    <t>Bank</t>
-  </si>
-  <si>
-    <t>Equipment</t>
-  </si>
-  <si>
-    <t>CPJ</t>
-  </si>
-  <si>
     <t>EQUIPMENT</t>
-  </si>
-  <si>
-    <t>Rent expense</t>
-  </si>
-  <si>
-    <t>Current income</t>
-  </si>
-  <si>
-    <t>Wages</t>
   </si>
   <si>
     <t>WAGES</t>
   </si>
   <si>
-    <t>Drawings</t>
-  </si>
-  <si>
     <t>DRAWINGS</t>
-  </si>
-  <si>
-    <t>Water and Electricity</t>
   </si>
   <si>
     <t>WATER AND ELECTRICITY</t>
   </si>
   <si>
-    <t>Telephone</t>
-  </si>
-  <si>
     <t>TELEPHONE</t>
   </si>
   <si>
-    <t>Stationery</t>
-  </si>
-  <si>
     <t>STATIONERY</t>
-  </si>
-  <si>
-    <t>Balance</t>
-  </si>
-  <si>
-    <t>c/d</t>
-  </si>
-  <si>
-    <t>Mar</t>
-  </si>
-  <si>
-    <t>b/d</t>
   </si>
 </sst>
 </file>
@@ -553,15 +499,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -574,6 +519,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -583,14 +537,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -910,8 +856,8 @@
   </sheetPr>
   <dimension ref="A2:W83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="200" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="75" workbookViewId="0">
+      <selection activeCell="R68" sqref="N68:R68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -937,71 +883,71 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" ht="34" x14ac:dyDescent="0.4">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
     </row>
     <row r="5" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:23" ht="25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="29"/>
-      <c r="N6" s="27" t="s">
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="34"/>
+      <c r="N6" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="28"/>
-      <c r="S6" s="28"/>
-      <c r="T6" s="28"/>
-      <c r="U6" s="28"/>
-      <c r="V6" s="28"/>
-      <c r="W6" s="29"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="33"/>
+      <c r="S6" s="33"/>
+      <c r="T6" s="33"/>
+      <c r="U6" s="33"/>
+      <c r="V6" s="33"/>
+      <c r="W6" s="34"/>
     </row>
     <row r="7" spans="1:23" ht="25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="32"/>
-      <c r="N7" s="30" t="s">
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="40"/>
+      <c r="N7" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="31"/>
-      <c r="T7" s="31"/>
-      <c r="U7" s="31"/>
-      <c r="V7" s="31"/>
-      <c r="W7" s="32"/>
+      <c r="O7" s="39"/>
+      <c r="P7" s="39"/>
+      <c r="Q7" s="39"/>
+      <c r="R7" s="39"/>
+      <c r="S7" s="39"/>
+      <c r="T7" s="39"/>
+      <c r="U7" s="39"/>
+      <c r="V7" s="39"/>
+      <c r="W7" s="40"/>
     </row>
     <row r="8" spans="1:23" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="19"/>
@@ -1026,30 +972,30 @@
       <c r="W8" s="21"/>
     </row>
     <row r="9" spans="1:23" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="25"/>
-      <c r="N9" s="23" t="s">
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="37"/>
+      <c r="N9" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="24"/>
-      <c r="S9" s="24"/>
-      <c r="T9" s="24"/>
-      <c r="U9" s="24"/>
-      <c r="V9" s="24"/>
-      <c r="W9" s="25"/>
+      <c r="O9" s="36"/>
+      <c r="P9" s="36"/>
+      <c r="Q9" s="36"/>
+      <c r="R9" s="36"/>
+      <c r="S9" s="36"/>
+      <c r="T9" s="36"/>
+      <c r="U9" s="36"/>
+      <c r="V9" s="36"/>
+      <c r="W9" s="37"/>
     </row>
     <row r="10" spans="1:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -1116,128 +1062,60 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="9">
-        <v>1</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="33">
-        <v>1000000</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="9">
-        <v>4</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="K11" s="34">
-        <v>800000</v>
-      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="24"/>
       <c r="N11" s="8"/>
       <c r="O11" s="9"/>
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
       <c r="R11" s="16"/>
-      <c r="S11" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="T11" s="9">
-        <v>6</v>
-      </c>
-      <c r="U11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="V11" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="W11" s="34">
-        <v>112500</v>
-      </c>
+      <c r="S11" s="13"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="24"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B12" s="3"/>
-      <c r="C12" s="2">
-        <v>6</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="36">
-        <v>112500</v>
-      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="26"/>
       <c r="G12" s="14"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K12" s="35">
-        <v>35000</v>
-      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="25"/>
       <c r="N12" s="3"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="17"/>
       <c r="S12" s="14"/>
-      <c r="T12" s="2">
-        <v>19</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="V12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="W12" s="35">
-        <v>10120</v>
-      </c>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="25"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B13" s="3"/>
-      <c r="C13" s="2">
-        <v>19</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="36">
-        <v>10120</v>
-      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="26"/>
       <c r="G13" s="14"/>
-      <c r="H13" s="2">
-        <v>10</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K13" s="35">
-        <v>3000</v>
-      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="25"/>
       <c r="N13" s="3"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
@@ -1252,28 +1130,14 @@
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B14" s="3"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="36">
-        <v>200000</v>
-      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="26"/>
       <c r="G14" s="14"/>
-      <c r="H14" s="2">
-        <v>12</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" s="35">
-        <v>19000</v>
-      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="25"/>
       <c r="N14" s="3"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
@@ -1292,18 +1156,10 @@
       <c r="E15" s="2"/>
       <c r="F15" s="17"/>
       <c r="G15" s="14"/>
-      <c r="H15" s="2">
-        <v>15</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K15" s="35">
-        <v>6000</v>
-      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="25"/>
       <c r="N15" s="3"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
@@ -1322,18 +1178,10 @@
       <c r="E16" s="2"/>
       <c r="F16" s="17"/>
       <c r="G16" s="14"/>
-      <c r="H16" s="2">
-        <v>16</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K16" s="35">
-        <v>2300</v>
-      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="25"/>
       <c r="N16" s="3"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
@@ -1352,18 +1200,10 @@
       <c r="E17" s="2"/>
       <c r="F17" s="17"/>
       <c r="G17" s="14"/>
-      <c r="H17" s="2">
-        <v>21</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K17" s="35">
-        <v>1890</v>
-      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="25"/>
       <c r="N17" s="5"/>
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
@@ -1382,18 +1222,10 @@
       <c r="E18" s="2"/>
       <c r="F18" s="17"/>
       <c r="G18" s="14"/>
-      <c r="H18" s="2">
-        <v>23</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K18" s="4">
-        <v>610</v>
-      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="4"/>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
@@ -1402,18 +1234,10 @@
       <c r="E19" s="2"/>
       <c r="F19" s="17"/>
       <c r="G19" s="14"/>
-      <c r="H19" s="2">
-        <v>25</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K19" s="35">
-        <v>3000</v>
-      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="25"/>
     </row>
     <row r="20" spans="2:23" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3"/>
@@ -1422,19 +1246,10 @@
       <c r="E20" s="2"/>
       <c r="F20" s="17"/>
       <c r="G20" s="14"/>
-      <c r="H20" s="2">
-        <v>28</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K20" s="35">
-        <f>K21-SUM(K11:K19)</f>
-        <v>451820</v>
-      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="25"/>
       <c r="N20" s="22"/>
       <c r="O20" s="22"/>
       <c r="P20" s="22"/>
@@ -1451,53 +1266,36 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="37">
-        <f>SUM(F11:F14)</f>
-        <v>1322620</v>
-      </c>
+      <c r="F21" s="27"/>
       <c r="G21" s="14"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="39">
-        <f>F21</f>
-        <v>1322620</v>
-      </c>
-      <c r="N21" s="23" t="s">
+      <c r="K21" s="29"/>
+      <c r="N21" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="24"/>
-      <c r="S21" s="24"/>
-      <c r="T21" s="24"/>
-      <c r="U21" s="24"/>
-      <c r="V21" s="24"/>
-      <c r="W21" s="25"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="36"/>
+      <c r="Q21" s="36"/>
+      <c r="R21" s="36"/>
+      <c r="S21" s="36"/>
+      <c r="T21" s="36"/>
+      <c r="U21" s="36"/>
+      <c r="V21" s="36"/>
+      <c r="W21" s="37"/>
     </row>
     <row r="22" spans="2:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="6">
-        <v>1</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" s="40">
-        <f>K20</f>
-        <v>451820</v>
-      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="30"/>
       <c r="G22" s="15"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
-      <c r="K22" s="38"/>
+      <c r="K22" s="28"/>
       <c r="N22" s="11" t="s">
         <v>5</v>
       </c>
@@ -1542,18 +1340,18 @@
       <c r="W23" s="10"/>
     </row>
     <row r="24" spans="2:23" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="25"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="37"/>
       <c r="N24" s="3"/>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
@@ -1613,21 +1411,11 @@
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="16"/>
-      <c r="G26" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H26" s="9">
-        <v>1</v>
-      </c>
-      <c r="I26" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J26" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K26" s="34">
-        <v>1000000</v>
-      </c>
+      <c r="G26" s="13"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="24"/>
       <c r="N26" s="3"/>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
@@ -1646,18 +1434,10 @@
       <c r="E27" s="2"/>
       <c r="F27" s="17"/>
       <c r="G27" s="14"/>
-      <c r="H27" s="2">
-        <v>19</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K27" s="35">
-        <v>200000</v>
-      </c>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="25"/>
       <c r="N27" s="3"/>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
@@ -1736,18 +1516,18 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="4"/>
-      <c r="N31" s="23" t="s">
+      <c r="N31" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="O31" s="24"/>
-      <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
-      <c r="R31" s="24"/>
-      <c r="S31" s="24"/>
-      <c r="T31" s="24"/>
-      <c r="U31" s="24"/>
-      <c r="V31" s="24"/>
-      <c r="W31" s="25"/>
+      <c r="O31" s="36"/>
+      <c r="P31" s="36"/>
+      <c r="Q31" s="36"/>
+      <c r="R31" s="36"/>
+      <c r="S31" s="36"/>
+      <c r="T31" s="36"/>
+      <c r="U31" s="36"/>
+      <c r="V31" s="36"/>
+      <c r="W31" s="37"/>
     </row>
     <row r="32" spans="2:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
@@ -1792,21 +1572,11 @@
       </c>
     </row>
     <row r="33" spans="2:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="N33" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="O33" s="9">
-        <v>4</v>
-      </c>
-      <c r="P33" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q33" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="R33" s="33">
-        <v>35000</v>
-      </c>
+      <c r="N33" s="8"/>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="9"/>
+      <c r="R33" s="23"/>
       <c r="S33" s="13"/>
       <c r="T33" s="9"/>
       <c r="U33" s="9"/>
@@ -1814,18 +1584,18 @@
       <c r="W33" s="10"/>
     </row>
     <row r="34" spans="2:23" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="24"/>
-      <c r="K34" s="25"/>
+      <c r="B34" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="36"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="36"/>
+      <c r="I34" s="36"/>
+      <c r="J34" s="36"/>
+      <c r="K34" s="37"/>
       <c r="N34" s="3"/>
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
@@ -1880,21 +1650,11 @@
       <c r="W35" s="4"/>
     </row>
     <row r="36" spans="2:23" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" s="9">
-        <v>4</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F36" s="33">
-        <v>800000</v>
-      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="13"/>
       <c r="H36" s="9"/>
       <c r="I36" s="9"/>
@@ -1913,18 +1673,10 @@
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B37" s="3"/>
-      <c r="C37" s="2">
-        <v>12</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F37" s="36">
-        <v>19000</v>
-      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="26"/>
       <c r="G37" s="14"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
@@ -2008,18 +1760,18 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="4"/>
-      <c r="N41" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="O41" s="24"/>
-      <c r="P41" s="24"/>
-      <c r="Q41" s="24"/>
-      <c r="R41" s="24"/>
-      <c r="S41" s="24"/>
-      <c r="T41" s="24"/>
-      <c r="U41" s="24"/>
-      <c r="V41" s="24"/>
-      <c r="W41" s="25"/>
+      <c r="N41" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="O41" s="36"/>
+      <c r="P41" s="36"/>
+      <c r="Q41" s="36"/>
+      <c r="R41" s="36"/>
+      <c r="S41" s="36"/>
+      <c r="T41" s="36"/>
+      <c r="U41" s="36"/>
+      <c r="V41" s="36"/>
+      <c r="W41" s="37"/>
     </row>
     <row r="42" spans="2:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B42" s="5"/>
@@ -2064,21 +1816,11 @@
       </c>
     </row>
     <row r="43" spans="2:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="N43" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="O43" s="9">
-        <v>10</v>
-      </c>
-      <c r="P43" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q43" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="R43" s="33">
-        <v>3000</v>
-      </c>
+      <c r="N43" s="8"/>
+      <c r="O43" s="9"/>
+      <c r="P43" s="9"/>
+      <c r="Q43" s="9"/>
+      <c r="R43" s="23"/>
       <c r="S43" s="13"/>
       <c r="T43" s="9"/>
       <c r="U43" s="9"/>
@@ -2086,31 +1828,23 @@
       <c r="W43" s="10"/>
     </row>
     <row r="44" spans="2:23" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24"/>
-      <c r="H44" s="24"/>
-      <c r="I44" s="24"/>
-      <c r="J44" s="24"/>
-      <c r="K44" s="25"/>
+      <c r="B44" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="36"/>
+      <c r="G44" s="36"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
+      <c r="K44" s="37"/>
       <c r="N44" s="3"/>
-      <c r="O44" s="2">
-        <v>25</v>
-      </c>
-      <c r="P44" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q44" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="R44" s="36">
-        <v>3000</v>
-      </c>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+      <c r="R44" s="26"/>
       <c r="S44" s="14"/>
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
@@ -2160,21 +1894,11 @@
       <c r="W45" s="4"/>
     </row>
     <row r="46" spans="2:23" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C46" s="9">
-        <v>15</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F46" s="33">
-        <v>6000</v>
-      </c>
+      <c r="B46" s="8"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="23"/>
       <c r="G46" s="13"/>
       <c r="H46" s="9"/>
       <c r="I46" s="9"/>
@@ -2280,18 +2004,18 @@
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="4"/>
-      <c r="N51" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="O51" s="24"/>
-      <c r="P51" s="24"/>
-      <c r="Q51" s="24"/>
-      <c r="R51" s="24"/>
-      <c r="S51" s="24"/>
-      <c r="T51" s="24"/>
-      <c r="U51" s="24"/>
-      <c r="V51" s="24"/>
-      <c r="W51" s="25"/>
+      <c r="N51" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="O51" s="36"/>
+      <c r="P51" s="36"/>
+      <c r="Q51" s="36"/>
+      <c r="R51" s="36"/>
+      <c r="S51" s="36"/>
+      <c r="T51" s="36"/>
+      <c r="U51" s="36"/>
+      <c r="V51" s="36"/>
+      <c r="W51" s="37"/>
     </row>
     <row r="52" spans="2:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B52" s="5"/>
@@ -2336,21 +2060,11 @@
       </c>
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="N53" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="O53" s="2">
-        <v>16</v>
-      </c>
-      <c r="P53" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q53" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="R53" s="36">
-        <v>2300</v>
-      </c>
+      <c r="N53" s="3"/>
+      <c r="O53" s="2"/>
+      <c r="P53" s="2"/>
+      <c r="Q53" s="2"/>
+      <c r="R53" s="26"/>
       <c r="S53" s="14"/>
       <c r="T53" s="2"/>
       <c r="U53" s="2"/>
@@ -2370,16 +2084,16 @@
       <c r="W54" s="4"/>
     </row>
     <row r="55" spans="2:23" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="23"/>
-      <c r="C55" s="24"/>
-      <c r="D55" s="24"/>
-      <c r="E55" s="24"/>
-      <c r="F55" s="24"/>
-      <c r="G55" s="24"/>
-      <c r="H55" s="24"/>
-      <c r="I55" s="24"/>
-      <c r="J55" s="24"/>
-      <c r="K55" s="25"/>
+      <c r="B55" s="35"/>
+      <c r="C55" s="36"/>
+      <c r="D55" s="36"/>
+      <c r="E55" s="36"/>
+      <c r="F55" s="36"/>
+      <c r="G55" s="36"/>
+      <c r="H55" s="36"/>
+      <c r="I55" s="36"/>
+      <c r="J55" s="36"/>
+      <c r="K55" s="37"/>
       <c r="N55" s="3"/>
       <c r="O55" s="2"/>
       <c r="P55" s="2"/>
@@ -2456,18 +2170,18 @@
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
       <c r="K58" s="4"/>
-      <c r="N58" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="O58" s="24"/>
-      <c r="P58" s="24"/>
-      <c r="Q58" s="24"/>
-      <c r="R58" s="24"/>
-      <c r="S58" s="24"/>
-      <c r="T58" s="24"/>
-      <c r="U58" s="24"/>
-      <c r="V58" s="24"/>
-      <c r="W58" s="25"/>
+      <c r="N58" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="O58" s="36"/>
+      <c r="P58" s="36"/>
+      <c r="Q58" s="36"/>
+      <c r="R58" s="36"/>
+      <c r="S58" s="36"/>
+      <c r="T58" s="36"/>
+      <c r="U58" s="36"/>
+      <c r="V58" s="36"/>
+      <c r="W58" s="37"/>
     </row>
     <row r="59" spans="2:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B59" s="3"/>
@@ -2522,21 +2236,11 @@
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
       <c r="K60" s="7"/>
-      <c r="N60" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="O60" s="9">
-        <v>21</v>
-      </c>
-      <c r="P60" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q60" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="R60" s="33">
-        <v>1890</v>
-      </c>
+      <c r="N60" s="8"/>
+      <c r="O60" s="9"/>
+      <c r="P60" s="9"/>
+      <c r="Q60" s="9"/>
+      <c r="R60" s="23"/>
       <c r="S60" s="13"/>
       <c r="T60" s="9"/>
       <c r="U60" s="9"/>
@@ -2556,16 +2260,16 @@
       <c r="W61" s="4"/>
     </row>
     <row r="62" spans="2:23" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="23"/>
-      <c r="C62" s="24"/>
-      <c r="D62" s="24"/>
-      <c r="E62" s="24"/>
-      <c r="F62" s="24"/>
-      <c r="G62" s="24"/>
-      <c r="H62" s="24"/>
-      <c r="I62" s="24"/>
-      <c r="J62" s="24"/>
-      <c r="K62" s="25"/>
+      <c r="B62" s="35"/>
+      <c r="C62" s="36"/>
+      <c r="D62" s="36"/>
+      <c r="E62" s="36"/>
+      <c r="F62" s="36"/>
+      <c r="G62" s="36"/>
+      <c r="H62" s="36"/>
+      <c r="I62" s="36"/>
+      <c r="J62" s="36"/>
+      <c r="K62" s="37"/>
       <c r="N62" s="3"/>
       <c r="O62" s="2"/>
       <c r="P62" s="2"/>
@@ -2664,18 +2368,18 @@
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
       <c r="K66" s="4"/>
-      <c r="N66" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="O66" s="24"/>
-      <c r="P66" s="24"/>
-      <c r="Q66" s="24"/>
-      <c r="R66" s="24"/>
-      <c r="S66" s="24"/>
-      <c r="T66" s="24"/>
-      <c r="U66" s="24"/>
-      <c r="V66" s="24"/>
-      <c r="W66" s="25"/>
+      <c r="N66" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="O66" s="36"/>
+      <c r="P66" s="36"/>
+      <c r="Q66" s="36"/>
+      <c r="R66" s="36"/>
+      <c r="S66" s="36"/>
+      <c r="T66" s="36"/>
+      <c r="U66" s="36"/>
+      <c r="V66" s="36"/>
+      <c r="W66" s="37"/>
     </row>
     <row r="67" spans="2:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B67" s="3"/>
@@ -2730,21 +2434,11 @@
       <c r="I68" s="6"/>
       <c r="J68" s="6"/>
       <c r="K68" s="7"/>
-      <c r="N68" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="O68" s="9">
-        <v>23</v>
-      </c>
-      <c r="P68" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q68" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="R68" s="16">
-        <v>610</v>
-      </c>
+      <c r="N68" s="8"/>
+      <c r="O68" s="9"/>
+      <c r="P68" s="9"/>
+      <c r="Q68" s="9"/>
+      <c r="R68" s="16"/>
       <c r="S68" s="13"/>
       <c r="T68" s="9"/>
       <c r="U68" s="9"/>
@@ -2764,16 +2458,16 @@
       <c r="W69" s="4"/>
     </row>
     <row r="70" spans="2:23" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="23"/>
-      <c r="C70" s="24"/>
-      <c r="D70" s="24"/>
-      <c r="E70" s="24"/>
-      <c r="F70" s="24"/>
-      <c r="G70" s="24"/>
-      <c r="H70" s="24"/>
-      <c r="I70" s="24"/>
-      <c r="J70" s="24"/>
-      <c r="K70" s="25"/>
+      <c r="B70" s="35"/>
+      <c r="C70" s="36"/>
+      <c r="D70" s="36"/>
+      <c r="E70" s="36"/>
+      <c r="F70" s="36"/>
+      <c r="G70" s="36"/>
+      <c r="H70" s="36"/>
+      <c r="I70" s="36"/>
+      <c r="J70" s="36"/>
+      <c r="K70" s="37"/>
       <c r="N70" s="3"/>
       <c r="O70" s="2"/>
       <c r="P70" s="2"/>
@@ -2872,16 +2566,16 @@
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
       <c r="K74" s="4"/>
-      <c r="N74" s="23"/>
-      <c r="O74" s="24"/>
-      <c r="P74" s="24"/>
-      <c r="Q74" s="24"/>
-      <c r="R74" s="24"/>
-      <c r="S74" s="24"/>
-      <c r="T74" s="24"/>
-      <c r="U74" s="24"/>
-      <c r="V74" s="24"/>
-      <c r="W74" s="25"/>
+      <c r="N74" s="35"/>
+      <c r="O74" s="36"/>
+      <c r="P74" s="36"/>
+      <c r="Q74" s="36"/>
+      <c r="R74" s="36"/>
+      <c r="S74" s="36"/>
+      <c r="T74" s="36"/>
+      <c r="U74" s="36"/>
+      <c r="V74" s="36"/>
+      <c r="W74" s="37"/>
     </row>
     <row r="75" spans="2:23" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B75" s="5"/>
@@ -2938,16 +2632,16 @@
       <c r="W76" s="10"/>
     </row>
     <row r="77" spans="2:23" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="23"/>
-      <c r="C77" s="24"/>
-      <c r="D77" s="24"/>
-      <c r="E77" s="24"/>
-      <c r="F77" s="24"/>
-      <c r="G77" s="24"/>
-      <c r="H77" s="24"/>
-      <c r="I77" s="24"/>
-      <c r="J77" s="24"/>
-      <c r="K77" s="25"/>
+      <c r="B77" s="35"/>
+      <c r="C77" s="36"/>
+      <c r="D77" s="36"/>
+      <c r="E77" s="36"/>
+      <c r="F77" s="36"/>
+      <c r="G77" s="36"/>
+      <c r="H77" s="36"/>
+      <c r="I77" s="36"/>
+      <c r="J77" s="36"/>
+      <c r="K77" s="37"/>
       <c r="N77" s="3"/>
       <c r="O77" s="2"/>
       <c r="P77" s="2"/>
@@ -3083,6 +2777,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B24:K24"/>
+    <mergeCell ref="B34:K34"/>
+    <mergeCell ref="B70:K70"/>
+    <mergeCell ref="B77:K77"/>
+    <mergeCell ref="N74:W74"/>
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="N6:W6"/>
     <mergeCell ref="N58:W58"/>
@@ -3099,11 +2798,6 @@
     <mergeCell ref="B6:K6"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="B9:K9"/>
-    <mergeCell ref="B24:K24"/>
-    <mergeCell ref="B34:K34"/>
-    <mergeCell ref="B70:K70"/>
-    <mergeCell ref="B77:K77"/>
-    <mergeCell ref="N74:W74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="68" fitToWidth="2" fitToHeight="4" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>